<commit_message>
System1 login and logout sequences
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IGNACIO\Documents\ProjetosGitHub\Calculate Client Security Hash\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IGNACIO\Documents\ProjetosGitHub\Calculate-Client-Security-Hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447FF71A-E3B1-4B5C-997F-FEF0D04C254F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6760A474-41A0-47D6-96C0-2F5691156589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -524,7 +524,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
SHA1 open and close sequences
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IGNACIO\Documents\ProjetosGitHub\Calculate-Client-Security-Hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6760A474-41A0-47D6-96C0-2F5691156589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEC4CE3-506F-4B0C-A230-1812C8BFCD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -524,7 +524,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
navigate and extract in work items
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IGNACIO\Documents\ProjetosGitHub\Calculate-Client-Security-Hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEC4CE3-506F-4B0C-A230-1812C8BFCD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B9F698-5EEE-4A52-A62C-B44E1CA34A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -524,7 +524,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
get Client information and adding sequences to main process
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IGNACIO\Documents\ProjetosGitHub\Calculate-Client-Security-Hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B9F698-5EEE-4A52-A62C-B44E1CA34A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99842CD-E6E2-44E6-A462-A5E00BEF4AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -524,7 +524,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>